<commit_message>
Translate newdir/test.xlsx in he_IL
100% translated source file: 'newdir/test.xlsx'
on 'he_IL'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_he_IL.xlsx
+++ b/Τranslations/test1_he_IL.xlsx
@@ -327,12 +327,12 @@
           <t>se</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="0" t="inlineStr">
         <is>
           <t>es</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="0" t="inlineStr">
         <is>
           <t>he_IL</t>
         </is>
@@ -344,37 +344,23 @@
           <t>test</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>test 1</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>test 1 fr</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>test de_DE</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>τεστ</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="H2" s="0" t="inlineStr"/>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>δοκιμασία</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="0" t="inlineStr">
         <is>
           <t>examen</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="0" t="inlineStr">
         <is>
           <t>בדיקה</t>
         </is>
@@ -386,23 +372,27 @@
           <t>example</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
         <is>
           <t>παράδειγμα</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" s="0" t="inlineStr">
         <is>
           <t>ejemplo</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" s="0" t="inlineStr">
         <is>
           <t>דוגמא</t>
         </is>
@@ -414,23 +404,27 @@
           <t>fish</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
         <is>
           <t>ψάρι</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" s="0" t="inlineStr">
         <is>
           <t>pez</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" s="0" t="inlineStr">
         <is>
           <t>דג</t>
         </is>

</xml_diff>

<commit_message>
Translate newdir/test.xlsx in he_IL [Manual Sync]
100% translated source file: 'newdir/test.xlsx'
on 'he_IL'.
</commit_message>
<xml_diff>
--- a/Τranslations/test1_he_IL.xlsx
+++ b/Τranslations/test1_he_IL.xlsx
@@ -364,7 +364,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -416,7 +416,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -468,7 +468,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>

</xml_diff>